<commit_message>
new changes as for new rail car color issue
</commit_message>
<xml_diff>
--- a/final_report/Trace_Report_CANOLA MEAL_initial.xlsx
+++ b/final_report/Trace_Report_CANOLA MEAL_initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rail car\final_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A67E9BA-8A59-4765-90B9-0E3827FBB1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46076396-1109-456F-86BD-D6486D0DC0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="3045" windowWidth="15375" windowHeight="7875"/>
+    <workbookView xWindow="2160" yWindow="1110" windowWidth="15375" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Test_format_trace" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="125">
   <si>
     <t>Initial</t>
   </si>
@@ -65,6 +65,36 @@
     <t>Destination City</t>
   </si>
   <si>
+    <t>BNSF</t>
+  </si>
+  <si>
+    <t>Not authorized to view shipment</t>
+  </si>
+  <si>
+    <t>ADMX</t>
+  </si>
+  <si>
+    <t>CHEYENNE</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>Arrive In-Transit</t>
+  </si>
+  <si>
+    <t>MNPNY2</t>
+  </si>
+  <si>
+    <t>JOHNSTOWN</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>TILX</t>
+  </si>
+  <si>
     <t>TRGX</t>
   </si>
   <si>
@@ -74,130 +104,130 @@
     <t>AB</t>
   </si>
   <si>
-    <t>Arrive In-Transit</t>
-  </si>
-  <si>
     <t>LOVELAND</t>
   </si>
   <si>
-    <t>CO</t>
+    <t>CEFX</t>
+  </si>
+  <si>
+    <t>CREWS</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>HKCKDE</t>
+  </si>
+  <si>
+    <t>AEX</t>
+  </si>
+  <si>
+    <t>DENVER</t>
+  </si>
+  <si>
+    <t>CRDX</t>
+  </si>
+  <si>
+    <t>CBFX</t>
+  </si>
+  <si>
+    <t>EAST WINONA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>HNTWKC</t>
+  </si>
+  <si>
+    <t>GACX</t>
+  </si>
+  <si>
+    <t>NDYX</t>
+  </si>
+  <si>
+    <t>SAMX</t>
+  </si>
+  <si>
+    <t>ENDERLIN</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Pulled from Cust</t>
+  </si>
+  <si>
+    <t>CITX</t>
+  </si>
+  <si>
+    <t>FURX</t>
+  </si>
+  <si>
+    <t>SHPX</t>
+  </si>
+  <si>
+    <t>GLENDO</t>
+  </si>
+  <si>
+    <t>HLAUDE</t>
+  </si>
+  <si>
+    <t>SMW</t>
+  </si>
+  <si>
+    <t>HUTCHINSON</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Placed Actual</t>
   </si>
   <si>
     <t>WFRX</t>
   </si>
   <si>
-    <t>DENVER</t>
-  </si>
-  <si>
-    <t>HKCKDE</t>
-  </si>
-  <si>
-    <t>BNSF</t>
-  </si>
-  <si>
-    <t>CEFX</t>
-  </si>
-  <si>
-    <t>TILX</t>
-  </si>
-  <si>
-    <t>DILWORTH</t>
+    <t>CGEX</t>
+  </si>
+  <si>
+    <t>KANSAS CITY</t>
+  </si>
+  <si>
+    <t>KELIM</t>
+  </si>
+  <si>
+    <t>Junction Received</t>
+  </si>
+  <si>
+    <t>NORTH PLATTE W</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>MALNP1</t>
+  </si>
+  <si>
+    <t>NORTHTOWN</t>
   </si>
   <si>
     <t>MN</t>
   </si>
   <si>
-    <t>YDIL30</t>
+    <t>HGFDNT</t>
+  </si>
+  <si>
+    <t>NOYES</t>
+  </si>
+  <si>
+    <t>Junction Delivery</t>
   </si>
   <si>
     <t>AOKX</t>
   </si>
   <si>
-    <t>GREELEY</t>
-  </si>
-  <si>
-    <t>Junction Delivery</t>
-  </si>
-  <si>
-    <t>GWR</t>
-  </si>
-  <si>
-    <t>JOHNSTOWN</t>
-  </si>
-  <si>
-    <t>ADMX</t>
-  </si>
-  <si>
-    <t>FURX</t>
-  </si>
-  <si>
-    <t>HOLCOMB</t>
-  </si>
-  <si>
-    <t>KS</t>
-  </si>
-  <si>
-    <t>Departure</t>
-  </si>
-  <si>
-    <t>Placed Actual</t>
-  </si>
-  <si>
-    <t>CRDX</t>
-  </si>
-  <si>
-    <t>AEX</t>
-  </si>
-  <si>
-    <t>KANSAS CITY</t>
-  </si>
-  <si>
-    <t>HNTWKC</t>
-  </si>
-  <si>
-    <t>LA SALLE</t>
-  </si>
-  <si>
-    <t>LDI601</t>
-  </si>
-  <si>
-    <t>LAUREL</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>HLAUDE</t>
-  </si>
-  <si>
-    <t>CBFX</t>
-  </si>
-  <si>
-    <t>LITTLETON</t>
-  </si>
-  <si>
-    <t>Junction Received</t>
-  </si>
-  <si>
-    <t>NDYX</t>
-  </si>
-  <si>
-    <t>MENDON</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>SMW</t>
-  </si>
-  <si>
-    <t>NORTHTOWN</t>
-  </si>
-  <si>
-    <t>HDILNT</t>
-  </si>
-  <si>
-    <t>NOYES</t>
+    <t>WINDSOR</t>
   </si>
   <si>
     <t>Gross Weight</t>
@@ -209,109 +239,175 @@
     <t>Net Weight</t>
   </si>
   <si>
-    <t>Description unknown, completed 06/15/2023 08:34:12 EDT, by WPJTOWN1.The search returned: 33 events.</t>
+    <t>Description unknown, completed 06/21/2023 08:44:42 EDT, by WPJTOWN1.The search returned: 55 events.</t>
   </si>
   <si>
     <t>Car_no</t>
   </si>
   <si>
+    <t>BNSF429803</t>
+  </si>
+  <si>
+    <t>ADMX52302</t>
+  </si>
+  <si>
+    <t>TILX55461</t>
+  </si>
+  <si>
+    <t>TRGX856777</t>
+  </si>
+  <si>
+    <t>CEFX360827</t>
+  </si>
+  <si>
+    <t>AEX9137</t>
+  </si>
+  <si>
+    <t>CRDX15622</t>
+  </si>
+  <si>
+    <t>CBFX354105</t>
+  </si>
+  <si>
+    <t>CEFX10602</t>
+  </si>
+  <si>
+    <t>GACX14628</t>
+  </si>
+  <si>
+    <t>NDYX849429</t>
+  </si>
+  <si>
+    <t>SAMX11304</t>
+  </si>
+  <si>
+    <t>TILX570086</t>
+  </si>
+  <si>
+    <t>ADMX52161</t>
+  </si>
+  <si>
+    <t>ADMX52184</t>
+  </si>
+  <si>
+    <t>ADMX52651</t>
+  </si>
+  <si>
+    <t>CBFX354076</t>
+  </si>
+  <si>
+    <t>CEFX12257</t>
+  </si>
+  <si>
+    <t>CEFX12648</t>
+  </si>
+  <si>
+    <t>CEFX71022</t>
+  </si>
+  <si>
+    <t>CITX702021</t>
+  </si>
+  <si>
+    <t>FURX855301</t>
+  </si>
+  <si>
+    <t>GACX14172</t>
+  </si>
+  <si>
+    <t>SHPX454918</t>
+  </si>
+  <si>
+    <t>TILX641448</t>
+  </si>
+  <si>
     <t>TRGX854465</t>
   </si>
   <si>
+    <t>SMW826975</t>
+  </si>
+  <si>
+    <t>CEFX360842</t>
+  </si>
+  <si>
+    <t>CEFX360825</t>
+  </si>
+  <si>
     <t>WFRX454037</t>
   </si>
   <si>
-    <t>CEFX360825</t>
+    <t>CGEX1808</t>
+  </si>
+  <si>
+    <t>CITX701950</t>
+  </si>
+  <si>
+    <t>SAMX11324</t>
+  </si>
+  <si>
+    <t>SAMX11428</t>
   </si>
   <si>
     <t>TILX570277</t>
   </si>
   <si>
+    <t>FURX855176</t>
+  </si>
+  <si>
+    <t>FURX855178</t>
+  </si>
+  <si>
+    <t>TILX54219</t>
+  </si>
+  <si>
+    <t>TILX55662</t>
+  </si>
+  <si>
+    <t>WFRX454142</t>
+  </si>
+  <si>
+    <t>FURX855954</t>
+  </si>
+  <si>
+    <t>FURX855161</t>
+  </si>
+  <si>
+    <t>TRGX854637</t>
+  </si>
+  <si>
+    <t>ADMX560013</t>
+  </si>
+  <si>
+    <t>AEX8897</t>
+  </si>
+  <si>
+    <t>AEX8984</t>
+  </si>
+  <si>
+    <t>CEFX319870</t>
+  </si>
+  <si>
+    <t>TILX54208</t>
+  </si>
+  <si>
+    <t>FURX855173</t>
+  </si>
+  <si>
+    <t>FURX855156</t>
+  </si>
+  <si>
+    <t>AOKX854156</t>
+  </si>
+  <si>
+    <t>ADMX7079</t>
+  </si>
+  <si>
+    <t>TILX54177</t>
+  </si>
+  <si>
+    <t>ADMX54089</t>
+  </si>
+  <si>
     <t>AOKX854300</t>
-  </si>
-  <si>
-    <t>ADMX54089</t>
-  </si>
-  <si>
-    <t>TILX54177</t>
-  </si>
-  <si>
-    <t>ADMX7079</t>
-  </si>
-  <si>
-    <t>AOKX854156</t>
-  </si>
-  <si>
-    <t>FURX855161</t>
-  </si>
-  <si>
-    <t>TILX55566</t>
-  </si>
-  <si>
-    <t>CEFX360842</t>
-  </si>
-  <si>
-    <t>CRDX15011</t>
-  </si>
-  <si>
-    <t>ADMX63946</t>
-  </si>
-  <si>
-    <t>AEX9137</t>
-  </si>
-  <si>
-    <t>CRDX15622</t>
-  </si>
-  <si>
-    <t>FURX855954</t>
-  </si>
-  <si>
-    <t>TILX54219</t>
-  </si>
-  <si>
-    <t>TILX55662</t>
-  </si>
-  <si>
-    <t>WFRX454142</t>
-  </si>
-  <si>
-    <t>TRGX854637</t>
-  </si>
-  <si>
-    <t>CBFX490506</t>
-  </si>
-  <si>
-    <t>CBFX490552</t>
-  </si>
-  <si>
-    <t>TILX55148</t>
-  </si>
-  <si>
-    <t>TILX55449</t>
-  </si>
-  <si>
-    <t>TILX55811</t>
-  </si>
-  <si>
-    <t>FURX855169</t>
-  </si>
-  <si>
-    <t>NDYX841938</t>
-  </si>
-  <si>
-    <t>CEFX360827</t>
-  </si>
-  <si>
-    <t>SMW826975</t>
-  </si>
-  <si>
-    <t>FURX855156</t>
-  </si>
-  <si>
-    <t>FURX855176</t>
-  </si>
-  <si>
-    <t>FURX855178</t>
   </si>
 </sst>
 </file>
@@ -1152,17 +1248,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O35"/>
+      <selection activeCell="O3" sqref="O3:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1200,16 +1296,16 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1217,427 +1313,397 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>854465</v>
+        <v>429803</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>2256</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3">
-        <v>285676</v>
-      </c>
-      <c r="M3">
-        <v>63000</v>
-      </c>
-      <c r="N3">
-        <v>222676</v>
+      <c r="L3" t="s">
+        <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>52302</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>2100</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>454037</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>303</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L4">
-        <v>229086</v>
+        <v>204550</v>
       </c>
       <c r="M4">
-        <v>63700</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>165386</v>
+        <v>204550</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>55461</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="B5">
-        <v>360825</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G5">
+        <v>2100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>303</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L5">
-        <v>280078</v>
+        <v>214550</v>
       </c>
       <c r="M5">
-        <v>68300</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>211778</v>
+        <v>214550</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>856777</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
-        <v>570277</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="G6">
-        <v>418</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L6">
-        <v>236304</v>
+        <v>284574</v>
       </c>
       <c r="M6">
-        <v>66400</v>
+        <v>60000</v>
       </c>
       <c r="N6">
-        <v>169904</v>
+        <v>224574</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>360827</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="B7">
-        <v>854300</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>601</v>
+      </c>
+      <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>1609</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L7">
-        <v>183100</v>
+        <v>283496</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>68100</v>
       </c>
       <c r="N7">
-        <v>183100</v>
+        <v>215396</v>
       </c>
       <c r="O7" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>54089</v>
+        <v>9137</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <v>1259</v>
+      </c>
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>1609</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L8">
-        <v>214900</v>
+        <v>265958</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>70600</v>
       </c>
       <c r="N8">
-        <v>214900</v>
+        <v>195358</v>
       </c>
       <c r="O8" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>54177</v>
+        <v>15622</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>1259</v>
+      </c>
+      <c r="H9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>1609</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>27</v>
       </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L9">
-        <v>207550</v>
+        <v>280567</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>67200</v>
       </c>
       <c r="N9">
-        <v>207550</v>
+        <v>213367</v>
       </c>
       <c r="O9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>7079</v>
+        <v>354105</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>730</v>
+      </c>
+      <c r="H10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>11</v>
-      </c>
-      <c r="G10">
-        <v>1609</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L10">
-        <v>201950</v>
+        <v>251100</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>63000</v>
       </c>
       <c r="N10">
-        <v>201950</v>
+        <v>188100</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
-        <v>854156</v>
+        <v>10602</v>
       </c>
       <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>730</v>
+      </c>
+      <c r="H11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>1609</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L11">
-        <v>195150</v>
+        <v>251300</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>62900</v>
       </c>
       <c r="N11">
-        <v>195150</v>
+        <v>188400</v>
       </c>
       <c r="O11" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>855161</v>
+        <v>14628</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
@@ -1649,304 +1715,307 @@
         <v>6</v>
       </c>
       <c r="F12">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G12">
-        <v>702</v>
+        <v>730</v>
       </c>
       <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L12">
-        <v>226450</v>
+        <v>247900</v>
       </c>
       <c r="M12">
-        <v>60500</v>
+        <v>64600</v>
       </c>
       <c r="N12">
-        <v>165950</v>
+        <v>183300</v>
       </c>
       <c r="O12" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>849429</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
         <v>21</v>
       </c>
-      <c r="B13">
-        <v>55566</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-      <c r="F13">
-        <v>8</v>
-      </c>
       <c r="G13">
-        <v>1611</v>
+        <v>730</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L13">
-        <v>198400</v>
+        <v>266500</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>63100</v>
       </c>
       <c r="N13">
-        <v>198400</v>
+        <v>203400</v>
       </c>
       <c r="O13" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>360842</v>
+        <v>11304</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E14">
         <v>6</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G14">
-        <v>1608</v>
+        <v>730</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
       </c>
       <c r="J14" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L14">
-        <v>283996</v>
+        <v>264900</v>
       </c>
       <c r="M14">
-        <v>68100</v>
+        <v>62500</v>
       </c>
       <c r="N14">
-        <v>215896</v>
+        <v>202400</v>
       </c>
       <c r="O14" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>15011</v>
+        <v>570086</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E15">
         <v>6</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G15">
-        <v>1608</v>
+        <v>730</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L15">
-        <v>274319</v>
+        <v>251050</v>
       </c>
       <c r="M15">
-        <v>69400</v>
+        <v>63400</v>
       </c>
       <c r="N15">
-        <v>204919</v>
+        <v>187650</v>
       </c>
       <c r="O15" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>63946</v>
+        <v>52161</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E16">
         <v>6</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G16">
-        <v>1305</v>
+        <v>1420</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L16">
-        <v>198950</v>
+        <v>253850</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>62900</v>
       </c>
       <c r="N16">
-        <v>198950</v>
+        <v>190950</v>
       </c>
       <c r="O16" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>9137</v>
+        <v>52184</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E17">
         <v>6</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G17">
-        <v>756</v>
+        <v>1415</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J17" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L17">
-        <v>265958</v>
+        <v>284900</v>
       </c>
       <c r="M17">
-        <v>70600</v>
+        <v>69300</v>
       </c>
       <c r="N17">
-        <v>195358</v>
+        <v>215600</v>
       </c>
       <c r="O17" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>15622</v>
+        <v>52651</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E18">
         <v>6</v>
       </c>
       <c r="F18">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G18">
-        <v>756</v>
+        <v>1415</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L18">
-        <v>280567</v>
+        <v>250650</v>
       </c>
       <c r="M18">
-        <v>67200</v>
+        <v>61100</v>
       </c>
       <c r="N18">
-        <v>213367</v>
+        <v>189550</v>
       </c>
       <c r="O18" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1954,798 +2023,1769 @@
         <v>31</v>
       </c>
       <c r="B19">
-        <v>855954</v>
+        <v>354076</v>
       </c>
       <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>1420</v>
+      </c>
+      <c r="H19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19">
-        <v>6</v>
-      </c>
-      <c r="F19">
-        <v>14</v>
-      </c>
-      <c r="G19">
-        <v>1501</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>41</v>
-      </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L19">
-        <v>216100</v>
+        <v>249300</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>61900</v>
       </c>
       <c r="N19">
-        <v>216100</v>
+        <v>187400</v>
       </c>
       <c r="O19" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>54219</v>
+        <v>12257</v>
       </c>
       <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>1420</v>
+      </c>
+      <c r="H20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>14</v>
-      </c>
-      <c r="G20">
-        <v>1501</v>
-      </c>
-      <c r="H20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" t="s">
-        <v>41</v>
-      </c>
       <c r="J20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L20">
-        <v>209950</v>
+        <v>254150</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>61500</v>
       </c>
       <c r="N20">
-        <v>209950</v>
+        <v>192650</v>
       </c>
       <c r="O20" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B21">
-        <v>55662</v>
+        <v>12648</v>
       </c>
       <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>1415</v>
+      </c>
+      <c r="H21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21">
-        <v>14</v>
-      </c>
-      <c r="G21">
-        <v>1501</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" t="s">
-        <v>41</v>
-      </c>
       <c r="J21" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L21">
-        <v>212300</v>
+        <v>281350</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>69200</v>
       </c>
       <c r="N21">
-        <v>212300</v>
+        <v>212150</v>
       </c>
       <c r="O21" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>454142</v>
+        <v>71022</v>
       </c>
       <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>1420</v>
+      </c>
+      <c r="H22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22">
-        <v>14</v>
-      </c>
-      <c r="G22">
-        <v>1501</v>
-      </c>
-      <c r="H22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" t="s">
-        <v>41</v>
-      </c>
       <c r="J22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L22">
-        <v>219050</v>
+        <v>263250</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>62800</v>
       </c>
       <c r="N22">
-        <v>219050</v>
+        <v>200450</v>
       </c>
       <c r="O22" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>854637</v>
+        <v>702021</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G23">
-        <v>1437</v>
+        <v>1430</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L23">
-        <v>285434</v>
+        <v>251050</v>
       </c>
       <c r="M23">
-        <v>62800</v>
+        <v>62100</v>
       </c>
       <c r="N23">
-        <v>222634</v>
+        <v>188950</v>
       </c>
       <c r="O23" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24">
-        <v>490506</v>
+        <v>855301</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E24">
         <v>6</v>
       </c>
       <c r="F24">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G24">
-        <v>101</v>
+        <v>1425</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="J24" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L24">
-        <v>224300</v>
+        <v>252700</v>
       </c>
       <c r="M24">
-        <v>60900</v>
+        <v>62300</v>
       </c>
       <c r="N24">
-        <v>163400</v>
+        <v>190400</v>
       </c>
       <c r="O24" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>490552</v>
+        <v>14172</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G25">
-        <v>101</v>
+        <v>1415</v>
       </c>
       <c r="H25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="J25" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L25">
-        <v>222600</v>
+        <v>254150</v>
       </c>
       <c r="M25">
-        <v>60700</v>
+        <v>62700</v>
       </c>
       <c r="N25">
-        <v>161900</v>
+        <v>191450</v>
       </c>
       <c r="O25" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B26">
-        <v>55148</v>
+        <v>454918</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E26">
         <v>6</v>
       </c>
       <c r="F26">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G26">
-        <v>101</v>
+        <v>1420</v>
       </c>
       <c r="H26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L26">
-        <v>230400</v>
+        <v>238072</v>
       </c>
       <c r="M26">
-        <v>63700</v>
+        <v>67800</v>
       </c>
       <c r="N26">
-        <v>166700</v>
+        <v>170272</v>
       </c>
       <c r="O26" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27">
-        <v>55449</v>
+        <v>641448</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G27">
-        <v>101</v>
+        <v>1425</v>
       </c>
       <c r="H27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="J27" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K27" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L27">
-        <v>226750</v>
+        <v>237166</v>
       </c>
       <c r="M27">
-        <v>63700</v>
+        <v>67000</v>
       </c>
       <c r="N27">
-        <v>163050</v>
+        <v>170166</v>
       </c>
       <c r="O27" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>854465</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
         <v>21</v>
       </c>
-      <c r="B28">
-        <v>55811</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28">
-        <v>6</v>
-      </c>
-      <c r="F28">
-        <v>15</v>
-      </c>
       <c r="G28">
-        <v>101</v>
+        <v>613</v>
       </c>
       <c r="H28" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K28" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L28">
-        <v>225950</v>
+        <v>285676</v>
       </c>
       <c r="M28">
-        <v>63800</v>
+        <v>63000</v>
       </c>
       <c r="N28">
-        <v>162150</v>
+        <v>222676</v>
       </c>
       <c r="O28" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B29">
-        <v>855169</v>
+        <v>826975</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E29">
         <v>6</v>
       </c>
       <c r="F29">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G29">
-        <v>1045</v>
+        <v>357</v>
       </c>
       <c r="H29" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J29" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K29" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L29">
-        <v>239535</v>
+        <v>208106</v>
       </c>
       <c r="M29">
-        <v>60300</v>
+        <v>63400</v>
       </c>
       <c r="N29">
-        <v>179235</v>
+        <v>144706</v>
       </c>
       <c r="O29" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>841938</v>
+        <v>360842</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E30">
         <v>6</v>
       </c>
       <c r="F30">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <v>1428</v>
+        <v>1608</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L30">
-        <v>285905</v>
+        <v>283996</v>
       </c>
       <c r="M30">
-        <v>61600</v>
+        <v>68100</v>
       </c>
       <c r="N30">
-        <v>224305</v>
+        <v>215896</v>
       </c>
       <c r="O30" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>360827</v>
+        <v>360825</v>
       </c>
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>17</v>
+      </c>
+      <c r="G31">
+        <v>1431</v>
+      </c>
+      <c r="H31" t="s">
         <v>49</v>
       </c>
-      <c r="D31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31">
-        <v>6</v>
-      </c>
-      <c r="F31">
-        <v>15</v>
-      </c>
-      <c r="G31">
-        <v>715</v>
-      </c>
-      <c r="H31" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" t="s">
-        <v>39</v>
-      </c>
       <c r="J31" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L31">
-        <v>283496</v>
+        <v>280078</v>
       </c>
       <c r="M31">
-        <v>68100</v>
+        <v>68300</v>
       </c>
       <c r="N31">
-        <v>215396</v>
+        <v>211778</v>
       </c>
       <c r="O31" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32">
-        <v>826975</v>
+        <v>454037</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E32">
         <v>6</v>
       </c>
       <c r="F32">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G32">
-        <v>200</v>
+        <v>1431</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J32" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K32" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L32">
-        <v>208106</v>
+        <v>229086</v>
       </c>
       <c r="M32">
-        <v>63400</v>
+        <v>63700</v>
       </c>
       <c r="N32">
-        <v>144706</v>
+        <v>165386</v>
       </c>
       <c r="O32" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B33">
-        <v>855156</v>
+        <v>1808</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="E33">
         <v>6</v>
       </c>
       <c r="F33">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G33">
-        <v>2311</v>
+        <v>411</v>
       </c>
       <c r="H33" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="J33" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K33" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L33">
-        <v>236536</v>
+        <v>226572</v>
       </c>
       <c r="M33">
-        <v>60400</v>
+        <v>61700</v>
       </c>
       <c r="N33">
-        <v>176136</v>
+        <v>164872</v>
       </c>
       <c r="O33" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B34">
-        <v>855176</v>
+        <v>701950</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="E34">
         <v>6</v>
       </c>
       <c r="F34">
+        <v>21</v>
+      </c>
+      <c r="G34">
+        <v>411</v>
+      </c>
+      <c r="H34" t="s">
         <v>15</v>
       </c>
-      <c r="G34">
-        <v>110</v>
-      </c>
-      <c r="H34" t="s">
-        <v>27</v>
-      </c>
       <c r="I34" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="J34" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L34">
-        <v>239890</v>
+        <v>239202</v>
       </c>
       <c r="M34">
-        <v>60500</v>
+        <v>69100</v>
       </c>
       <c r="N34">
-        <v>179390</v>
+        <v>170102</v>
       </c>
       <c r="O34" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B35">
+        <v>11324</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>21</v>
+      </c>
+      <c r="G35">
+        <v>411</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35">
+        <v>169960</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>169960</v>
+      </c>
+      <c r="O35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>11428</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>21</v>
+      </c>
+      <c r="G36">
+        <v>411</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36">
+        <v>228682</v>
+      </c>
+      <c r="M36">
+        <v>62700</v>
+      </c>
+      <c r="N36">
+        <v>165982</v>
+      </c>
+      <c r="O36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>570277</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>20</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37">
+        <v>236304</v>
+      </c>
+      <c r="M37">
+        <v>66400</v>
+      </c>
+      <c r="N37">
+        <v>169904</v>
+      </c>
+      <c r="O37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>855176</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <v>20</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38">
+        <v>239890</v>
+      </c>
+      <c r="M38">
+        <v>60500</v>
+      </c>
+      <c r="N38">
+        <v>179390</v>
+      </c>
+      <c r="O38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
         <v>855178</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39">
+        <v>6</v>
+      </c>
+      <c r="F39">
+        <v>20</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>34</v>
+      </c>
+      <c r="J39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39">
+        <v>237317</v>
+      </c>
+      <c r="M39">
+        <v>60300</v>
+      </c>
+      <c r="N39">
+        <v>177017</v>
+      </c>
+      <c r="O39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>54219</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40">
+        <v>19</v>
+      </c>
+      <c r="G40">
+        <v>1344</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40">
+        <v>209950</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>209950</v>
+      </c>
+      <c r="O40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>55662</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>19</v>
+      </c>
+      <c r="G41">
+        <v>1344</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41">
+        <v>212300</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>212300</v>
+      </c>
+      <c r="O41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>454142</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>19</v>
+      </c>
+      <c r="G42">
+        <v>1344</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42">
+        <v>219050</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>219050</v>
+      </c>
+      <c r="O42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>855954</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <v>19</v>
+      </c>
+      <c r="G43">
+        <v>1344</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43">
+        <v>216100</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>216100</v>
+      </c>
+      <c r="O43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>855161</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>19</v>
+      </c>
+      <c r="G44">
+        <v>1215</v>
+      </c>
+      <c r="H44" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35">
-        <v>6</v>
-      </c>
-      <c r="F35">
+      <c r="I44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" t="s">
+        <v>18</v>
+      </c>
+      <c r="L44">
+        <v>226450</v>
+      </c>
+      <c r="M44">
+        <v>60500</v>
+      </c>
+      <c r="N44">
+        <v>165950</v>
+      </c>
+      <c r="O44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>854637</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>19</v>
+      </c>
+      <c r="G45">
+        <v>1215</v>
+      </c>
+      <c r="H45" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" t="s">
+        <v>18</v>
+      </c>
+      <c r="L45">
+        <v>285434</v>
+      </c>
+      <c r="M45">
+        <v>62800</v>
+      </c>
+      <c r="N45">
+        <v>222634</v>
+      </c>
+      <c r="O45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>560013</v>
+      </c>
+      <c r="C46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>21</v>
+      </c>
+      <c r="G46">
+        <v>727</v>
+      </c>
+      <c r="H46" t="s">
         <v>15</v>
       </c>
-      <c r="G35">
-        <v>110</v>
-      </c>
-      <c r="H35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="I46" t="s">
+        <v>57</v>
+      </c>
+      <c r="J46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" t="s">
+        <v>18</v>
+      </c>
+      <c r="L46">
+        <v>234728</v>
+      </c>
+      <c r="M46">
+        <v>60400</v>
+      </c>
+      <c r="N46">
+        <v>174328</v>
+      </c>
+      <c r="O46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47">
+        <v>8897</v>
+      </c>
+      <c r="C47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47">
+        <v>21</v>
+      </c>
+      <c r="G47">
+        <v>727</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>57</v>
+      </c>
+      <c r="J47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" t="s">
+        <v>18</v>
+      </c>
+      <c r="L47">
+        <v>236536</v>
+      </c>
+      <c r="M47">
+        <v>60400</v>
+      </c>
+      <c r="N47">
+        <v>176136</v>
+      </c>
+      <c r="O47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>8984</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48">
+        <v>6</v>
+      </c>
+      <c r="F48">
+        <v>21</v>
+      </c>
+      <c r="G48">
+        <v>727</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>57</v>
+      </c>
+      <c r="J48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48">
+        <v>222500</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>222500</v>
+      </c>
+      <c r="O48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>319870</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49">
+        <v>6</v>
+      </c>
+      <c r="F49">
+        <v>21</v>
+      </c>
+      <c r="G49">
+        <v>727</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J49" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49">
+        <v>218300</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>218300</v>
+      </c>
+      <c r="O49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>19</v>
       </c>
-      <c r="J35" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="B50">
+        <v>54208</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50">
+        <v>6</v>
+      </c>
+      <c r="F50">
+        <v>21</v>
+      </c>
+      <c r="G50">
+        <v>727</v>
+      </c>
+      <c r="H50" t="s">
         <v>15</v>
       </c>
-      <c r="L35">
-        <v>237317</v>
-      </c>
-      <c r="M35">
-        <v>60300</v>
-      </c>
-      <c r="N35">
-        <v>177017</v>
-      </c>
-      <c r="O35" t="s">
-        <v>92</v>
+      <c r="I50" t="s">
+        <v>57</v>
+      </c>
+      <c r="J50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50">
+        <v>217050</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>217050</v>
+      </c>
+      <c r="O50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51">
+        <v>855173</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51">
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <v>20</v>
+      </c>
+      <c r="G51">
+        <v>1954</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>60</v>
+      </c>
+      <c r="J51" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51">
+        <v>214900</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>214900</v>
+      </c>
+      <c r="O51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52">
+        <v>855156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>11</v>
+      </c>
+      <c r="G52">
+        <v>2311</v>
+      </c>
+      <c r="H52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52">
+        <v>220350</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>220350</v>
+      </c>
+      <c r="O52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53">
+        <v>854156</v>
+      </c>
+      <c r="C53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>19</v>
+      </c>
+      <c r="G53">
+        <v>1245</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53">
+        <v>195150</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>195150</v>
+      </c>
+      <c r="O53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54">
+        <v>7079</v>
+      </c>
+      <c r="C54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>19</v>
+      </c>
+      <c r="G54">
+        <v>1245</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54">
+        <v>201950</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>201950</v>
+      </c>
+      <c r="O54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55">
+        <v>54177</v>
+      </c>
+      <c r="C55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>19</v>
+      </c>
+      <c r="G55">
+        <v>1245</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="J55" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55">
+        <v>207550</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>207550</v>
+      </c>
+      <c r="O55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>54089</v>
+      </c>
+      <c r="C56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>19</v>
+      </c>
+      <c r="G56">
+        <v>1245</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56">
+        <v>214900</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>214900</v>
+      </c>
+      <c r="O56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
+        <v>854300</v>
+      </c>
+      <c r="C57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <v>19</v>
+      </c>
+      <c r="G57">
+        <v>1245</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57">
+        <v>183100</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>183100</v>
+      </c>
+      <c r="O57" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>